<commit_message>
updated CM version to 4.0.3.3
</commit_message>
<xml_diff>
--- a/commodity-application-modules/mobile-integration/API_URL.xlsx
+++ b/commodity-application-modules/mobile-integration/API_URL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mails\Documents\NetBeansProjects\files_and_resources\commodity-application-modules\mobile-integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B67D1B9-A7D4-49AD-BDE7-EB81372585FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7157CAF1-BE07-44AC-8455-34B6B08C1B17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3DE1FDCA-B5FE-4BED-8B32-FEF01A0E5E6B}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11325" xr2:uid="{3DE1FDCA-B5FE-4BED-8B32-FEF01A0E5E6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>API_SECTION</t>
   </si>
@@ -46,16 +46,36 @@
   </si>
   <si>
     <t>http://localhost:8080/openmrs/ws/rest/v2/inventory/consumption</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/openmrs/ws/rest/v2/inventory/stockOperation</t>
+  </si>
+  <si>
+    <t>Create any operation (receipt, distribution)</t>
+  </si>
+  <si>
+    <t>Complete Operation</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/openmrs/ws/rest/v2/inventory/stockOperation/{operation-id}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +98,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,16 +420,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D950CA-F4AA-4F76-8D54-5A3641FDE9AF}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="56.21875" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -425,8 +448,27 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{783E34C7-0FEE-4238-AC3C-53A4D1EF6D44}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>